<commit_message>
funcional con UpdateData.java y todo
</commit_message>
<xml_diff>
--- a/articulo.xlsx
+++ b/articulo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juang\Informatica\2DAM\Interfaz\ImportadorProductos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4580785C-96B2-4F45-9DF1-73C037ADB940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE5DF65-E70D-49F3-8D5E-5263DE309A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0 (2)" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="846">
   <si>
     <t>CODIGO</t>
   </si>
@@ -7481,9 +7481,6 @@
     <t>MARGEN</t>
   </si>
   <si>
-    <t>PIPAS GRANAINAS</t>
-  </si>
-  <si>
     <t>ARTICULO.IDENTIFICACION</t>
   </si>
   <si>
@@ -7560,6 +7557,12 @@
   </si>
   <si>
     <t>LINTARIF.SUBFAMILIA</t>
+  </si>
+  <si>
+    <t>PIPAS G</t>
+  </si>
+  <si>
+    <t>ALIMENTACIÓN</t>
   </si>
 </sst>
 </file>
@@ -8020,8 +8023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B87C35E-C910-4037-AD71-C165640BA7DE}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8062,10 +8065,10 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="G2" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="Z2" t="s">
-        <v>824</v>
+        <v>842</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -8184,93 +8187,93 @@
     </row>
     <row r="6" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>819</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>820</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>822</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>823</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>824</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>825</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>826</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>828</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>829</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>832</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>833</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>834</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>835</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>836</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>837</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="U6" s="1" t="s">
         <v>838</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="V6" s="1" t="s">
         <v>839</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="W6" s="1" t="s">
         <v>840</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>842</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>843</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>1</v>
+        <v>99999999</v>
       </c>
       <c r="B7" s="5">
-        <v>8421464006810</v>
+        <v>77777777</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>818</v>
+        <v>844</v>
       </c>
       <c r="D7" s="12">
         <v>21</v>
@@ -8279,36 +8282,35 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
+        <v>845</v>
       </c>
       <c r="H7" s="11">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
-        <v>794</v>
+      <c r="I7">
+        <v>3333</v>
       </c>
       <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" t="str">
-        <f>I7</f>
-        <v>PROVEEDOR1</v>
+        <f>IF(ISBLANK(A7),"",A7)</f>
+        <v>99999999</v>
+      </c>
+      <c r="K7">
+        <f>IF(ISBLANK(I7),"",I7)</f>
+        <v>3333</v>
       </c>
       <c r="L7">
-        <v>1111</v>
+        <v>988988</v>
       </c>
       <c r="M7" s="12">
         <v>400</v>
       </c>
-      <c r="N7" t="str">
-        <f>I7</f>
-        <v>PROVEEDOR1</v>
-      </c>
-      <c r="O7" t="s">
-        <v>794</v>
+      <c r="N7">
+        <f>IF(ISBLANK(I7),"",I7)</f>
+        <v>3333</v>
+      </c>
+      <c r="O7">
+        <f>IF(ISBLANK(I7),"",I7)</f>
+        <v>3333</v>
       </c>
       <c r="P7">
         <v>4</v>
@@ -8319,32 +8321,34 @@
       <c r="R7">
         <v>400</v>
       </c>
-      <c r="S7" t="s">
-        <v>794</v>
+      <c r="S7">
+        <f>IF(ISBLANK(I7),"",I7)</f>
+        <v>3333</v>
       </c>
       <c r="T7" s="2">
-        <f>A7</f>
-        <v>1</v>
+        <f>IF(ISBLANK(A7),"",A7)</f>
+        <v>99999999</v>
       </c>
       <c r="U7" t="s">
         <v>816</v>
       </c>
       <c r="V7">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="W7" s="13">
         <f>V7/(E7*0.01+1)</f>
-        <v>1.7355371900826448</v>
+        <v>1.2396694214876034</v>
       </c>
       <c r="X7" s="14">
         <v>0</v>
       </c>
       <c r="Y7" t="str">
-        <f>F7</f>
-        <v>Alimentación</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>12</v>
+        <f>IF(ISBLANK(F7),"",F7)</f>
+        <v>ALIMENTACIÓN</v>
+      </c>
+      <c r="Z7" t="str">
+        <f>IF(ISBLANK(G7),"",G7)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VERSION 2.0: FUNCIONALIDAD PERFECTA CON UN ÚNICO EXCEL Y ARCHIVO DE CONFIGURACIÓN
</commit_message>
<xml_diff>
--- a/articulo.xlsx
+++ b/articulo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juang\Informatica\2DAM\Interfaz\ImportadorProductos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE5DF65-E70D-49F3-8D5E-5263DE309A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EAC3A24-ACD9-4A52-8447-463C371CF7F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0 (2)" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2351" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="847">
   <si>
     <t>CODIGO</t>
   </si>
@@ -7559,10 +7559,13 @@
     <t>LINTARIF.SUBFAMILIA</t>
   </si>
   <si>
-    <t>PIPAS G</t>
-  </si>
-  <si>
     <t>ALIMENTACIÓN</t>
+  </si>
+  <si>
+    <t>MOCHILA 1</t>
+  </si>
+  <si>
+    <t>drogueria</t>
   </si>
 </sst>
 </file>
@@ -8023,8 +8026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B87C35E-C910-4037-AD71-C165640BA7DE}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8273,7 +8276,7 @@
         <v>77777777</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D7" s="12">
         <v>21</v>
@@ -8282,7 +8285,10 @@
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>845</v>
+        <v>844</v>
+      </c>
+      <c r="G7" t="s">
+        <v>846</v>
       </c>
       <c r="H7" s="11">
         <v>0</v>
@@ -8348,7 +8354,7 @@
       </c>
       <c r="Z7" t="str">
         <f>IF(ISBLANK(G7),"",G7)</f>
-        <v/>
+        <v>drogueria</v>
       </c>
     </row>
   </sheetData>

</xml_diff>